<commit_message>
Revert "ograniczenie zasiegu smyrania"
This reverts commit a5e3fe230e16ba8f3d64e540dbf67ad71c997b50.
</commit_message>
<xml_diff>
--- a/_game/lista rzeczy.xlsx
+++ b/_game/lista rzeczy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Beer-Garlic\_game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A81400F-9D23-4538-B8CF-FEB9A7E48482}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7C344C-9DCB-470D-9ED7-367E7226F5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CF51730E-8724-4ACC-87CE-382387E34EA0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>bugi:</t>
   </si>
@@ -53,9 +53,6 @@
     <t>dodanie kompletnego sterowania</t>
   </si>
   <si>
-    <t>fizyka, kiedy działa na gracza nie przesuwa kamery. Śledzenie gracza trzeba uzależnić od jego pozycji, a nie od eventu poruszania (chyba)</t>
-  </si>
-  <si>
     <t>cienie</t>
   </si>
   <si>
@@ -65,14 +62,67 @@
     <t>logo &lt;3</t>
   </si>
   <si>
-    <t>sterowanie, hover nad planszą zaznacza wszystkie pola nad jakimi jest myszka</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[ZROBIONE]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fizyka, kiedy działa na gracza nie przesuwa kamery. Śledzenie gracza trzeba uzależnić od jego pozycji, a nie od eventu poruszania (chyba)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[ZROBIONE]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sterowanie, hover nad planszą zaznacza wszystkie pola nad jakimi jest myszka</t>
+    </r>
+  </si>
+  <si>
+    <t>ekrany ładowania</t>
+  </si>
+  <si>
+    <t>generowanie świata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,8 +147,25 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +213,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -159,7 +232,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -169,8 +242,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -199,12 +273,16 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="20% — akcent 2" xfId="2" builtinId="34"/>
     <cellStyle name="20% — akcent 3" xfId="4" builtinId="38"/>
     <cellStyle name="20% — akcent 5" xfId="6" builtinId="46"/>
     <cellStyle name="20% — akcent 6" xfId="8" builtinId="50"/>
+    <cellStyle name="40% — akcent 6" xfId="9" builtinId="51"/>
     <cellStyle name="Akcent 2" xfId="1" builtinId="33"/>
     <cellStyle name="Akcent 3" xfId="3" builtinId="37"/>
     <cellStyle name="Akcent 5" xfId="5" builtinId="45"/>
@@ -524,7 +602,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,31 +631,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>6</v>
+      <c r="E2" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="C3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="C4" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>